<commit_message>
Add new files Fz_furnace_parts.xlsx and Fz_materials.xlsx
</commit_message>
<xml_diff>
--- a/float_zone_IKZ/Fz_materials.xlsx
+++ b/float_zone_IKZ/Fz_materials.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\brueckner\schemas\AreaA-data_modeling_and_schemas\float_zone_IKZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5973DAC2-775F-4790-9A94-F0913CEB826B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1C6E7E-31EE-4DF6-9970-CD43ED2D4242}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="dopant" sheetId="1" r:id="rId1"/>
-    <sheet name="feed rod" sheetId="3" r:id="rId2"/>
-    <sheet name="seed" sheetId="4" r:id="rId3"/>
-    <sheet name="gas" sheetId="2" r:id="rId4"/>
+    <sheet name="Dopant" sheetId="1" r:id="rId1"/>
+    <sheet name="Feed rod" sheetId="3" r:id="rId2"/>
+    <sheet name="Seed" sheetId="4" r:id="rId3"/>
+    <sheet name="Gas" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
   <si>
     <t># start Header</t>
   </si>
@@ -54,9 +54,6 @@
     <t># end Header</t>
   </si>
   <si>
-    <t>S013</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -84,27 +81,15 @@
     <t>Phosphine</t>
   </si>
   <si>
-    <t>dopant name</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
     <t>any important additional information (unstructured)</t>
   </si>
   <si>
     <t>name of gas</t>
   </si>
   <si>
-    <t>gas name</t>
-  </si>
-  <si>
     <t>Chemical formula of gas</t>
   </si>
   <si>
-    <t>gas type</t>
-  </si>
-  <si>
     <t>options: bottle, pipeline, other</t>
   </si>
   <si>
@@ -123,27 +108,9 @@
     <t>when was it delivered?</t>
   </si>
   <si>
-    <t>material type</t>
-  </si>
-  <si>
-    <t>diameter</t>
-  </si>
-  <si>
     <t>length</t>
   </si>
   <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>rod_surface</t>
-  </si>
-  <si>
-    <t>rod_pretreatment</t>
-  </si>
-  <si>
-    <t>rod_angle</t>
-  </si>
-  <si>
     <t>options: etched, raw, US cleaned</t>
   </si>
   <si>
@@ -195,9 +162,6 @@
     <t>name of seed</t>
   </si>
   <si>
-    <t>seed name</t>
-  </si>
-  <si>
     <t>ID of the seed</t>
   </si>
   <si>
@@ -205,6 +169,69 @@
   </si>
   <si>
     <t>seed orientation, options: &lt;111&gt;, &lt;100&gt;, other</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Gas Name</t>
+  </si>
+  <si>
+    <t>Gas source type</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Datetime</t>
+  </si>
+  <si>
+    <t>Seed orientation</t>
+  </si>
+  <si>
+    <t>Seed name</t>
+  </si>
+  <si>
+    <t>YYYY.MM.DD</t>
+  </si>
+  <si>
+    <t>Feed name</t>
+  </si>
+  <si>
+    <t>Material type</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Rod pretreatment</t>
+  </si>
+  <si>
+    <t>Rod surface</t>
+  </si>
+  <si>
+    <t>Rod angle</t>
+  </si>
+  <si>
+    <t>Length category?</t>
+  </si>
+  <si>
+    <t>Dopant name</t>
+  </si>
+  <si>
+    <t>PH3</t>
+  </si>
+  <si>
+    <t>alles super</t>
+  </si>
+  <si>
+    <t>Nitrogen</t>
+  </si>
+  <si>
+    <t>N2</t>
   </si>
 </sst>
 </file>
@@ -376,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -428,6 +455,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,14 +752,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -774,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>3</v>
@@ -887,19 +918,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -978,22 +1009,22 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1015,18 +1046,22 @@
       <c r="X9" s="6"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="A10" s="7"/>
       <c r="B10" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="18">
+        <v>45321</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
       <c r="I10" s="7"/>
@@ -1087,7 +1122,412 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U9" sqref="A1:U9"/>
+      <selection activeCell="T10" sqref="T10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+    </row>
+    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="S9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="8"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="10"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="N9:R9 T9">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$G9="aufgebraucht"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA2097F-63D0-4F80-9B47-E6DD22B24BDA}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1570,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>3</v>
@@ -1138,25 +1578,13 @@
       <c r="G2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>47</v>
-      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -1188,31 +1616,25 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>45</v>
-      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="N4" s="14"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -1249,39 +1671,29 @@
         <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
@@ -1340,169 +1752,63 @@
     </row>
     <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="O9" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q9" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="R9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="T9" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="10"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O9:S9">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$G9="aufgebraucht"</formula>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$F9="aufgebraucht"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA2097F-63D0-4F80-9B47-E6DD22B24BDA}">
-  <dimension ref="A1:T9"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA06E49-0219-42E2-BFF1-8F892FE889B5}">
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1521,12 +1827,8 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1540,29 +1842,25 @@
         <v>3</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1581,36 +1879,30 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="14"/>
+      <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1629,48 +1921,40 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-    </row>
-    <row r="6" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1689,12 +1973,8 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-    </row>
-    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1713,272 +1993,29 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-    </row>
-    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="17"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="O9:S9">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$G9="aufgebraucht"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA06E49-0219-42E2-BFF1-8F892FE889B5}">
-  <dimension ref="A1:P10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q12" sqref="A1:Q12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="6"/>
+        <v>50</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -1990,19 +2027,20 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
       <c r="I10" s="7"/>
       <c r="J10" s="8"/>
       <c r="K10" s="7"/>

</xml_diff>